<commit_message>
spo is ready and tested
</commit_message>
<xml_diff>
--- a/settings/event_id.xlsx
+++ b/settings/event_id.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem\PycharmProjects\RSKR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem\PycharmProjects\BG_RSKR\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DA7335-AA4B-4523-BFC4-EE6D70183FBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E63755A-2B6F-4FE8-8C29-9C6B43A7D227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23370" yWindow="2280" windowWidth="16680" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3285" yWindow="1710" windowWidth="21600" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t>EventID</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>15301, 15300</t>
+  </si>
+  <si>
+    <t>1511, 1515</t>
+  </si>
+  <si>
+    <t>Windows не может найти локальный профиль и выполняет вход в систему с временным профилем. Изменения Сделанные вами в этом профиле будут потеряны при выходе из системы.</t>
   </si>
 </sst>
 </file>
@@ -558,19 +564,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1014</v>
       </c>
@@ -586,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1309</v>
       </c>
@@ -594,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1310</v>
       </c>
@@ -602,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5612</v>
       </c>
@@ -610,7 +616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
@@ -618,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -626,7 +632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1000</v>
       </c>
@@ -634,7 +640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1026</v>
       </c>
@@ -642,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6666</v>
       </c>
@@ -650,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>16</v>
       </c>
@@ -658,7 +664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7034</v>
       </c>
@@ -666,7 +672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2004</v>
       </c>
@@ -674,7 +680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7023</v>
       </c>
@@ -682,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8233</v>
       </c>
@@ -690,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -698,7 +704,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>10004</v>
       </c>
@@ -706,7 +712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -714,7 +720,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -722,7 +728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1325</v>
       </c>
@@ -730,7 +736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>7032</v>
       </c>
@@ -738,7 +744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2004</v>
       </c>
@@ -746,7 +752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>5002</v>
       </c>
@@ -754,7 +760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1054</v>
       </c>
@@ -762,7 +768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>47</v>
       </c>
@@ -770,7 +776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>7023</v>
       </c>
@@ -778,7 +784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1030</v>
       </c>
@@ -786,7 +792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1008</v>
       </c>
@@ -794,7 +800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1023</v>
       </c>
@@ -802,7 +808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>10016</v>
       </c>
@@ -810,7 +816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>8208</v>
       </c>
@@ -818,7 +824,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>8200</v>
       </c>
@@ -826,7 +832,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2017</v>
       </c>
@@ -834,7 +840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>64</v>
       </c>
@@ -842,7 +848,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1002</v>
       </c>
@@ -850,7 +856,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4</v>
       </c>
@@ -858,7 +864,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1058</v>
       </c>
@@ -866,7 +872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>292</v>
       </c>
@@ -874,7 +880,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>7011</v>
       </c>
@@ -882,7 +888,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>7046</v>
       </c>
@@ -890,7 +896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>36</v>
       </c>
@@ -898,7 +904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1006</v>
       </c>
@@ -906,7 +912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>101</v>
       </c>
@@ -914,7 +920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>10400</v>
       </c>
@@ -922,7 +928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>50</v>
       </c>
@@ -930,7 +936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>0</v>
       </c>
@@ -938,7 +944,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>102</v>
       </c>
@@ -946,7 +952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>7009</v>
       </c>
@@ -954,7 +960,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>7031</v>
       </c>
@@ -962,7 +968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>10010</v>
       </c>
@@ -970,7 +976,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>1301</v>
       </c>
@@ -978,7 +984,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>513</v>
       </c>
@@ -986,7 +992,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>140</v>
       </c>
@@ -994,7 +1000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>58</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>5010</v>
       </c>
@@ -1018,7 +1024,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>5011</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>4879</v>
       </c>
@@ -1034,7 +1040,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>15</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>40960</v>
       </c>
@@ -1050,7 +1056,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>9009</v>
       </c>
@@ -1066,7 +1072,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>4879</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>8229</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>8228</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>1076</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>1067</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>6038</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>8015</v>
       </c>
@@ -1122,7 +1128,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>1129</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>10154</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>5719</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>6008</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>219</v>
       </c>
@@ -1162,7 +1168,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>63</v>
       </c>
@@ -1170,7 +1176,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>1534</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>68</v>
       </c>
@@ -1186,7 +1192,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>8016</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>16969</v>
       </c>
@@ -1202,7 +1208,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>10149</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>7022</v>
       </c>
@@ -1218,7 +1224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>1055</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>69</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>15021</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>2303</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>70</v>
       </c>
@@ -1258,7 +1264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>4</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>5</v>
       </c>
@@ -1274,7 +1280,16 @@
         <v>59</v>
       </c>
     </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>